<commit_message>
Remove “Table” and “TableColumn” from Summary sheet in DU_Evaluation.xlsx since they are not used
</commit_message>
<xml_diff>
--- a/assets/Template/ReportTemplate.xlsx
+++ b/assets/Template/ReportTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/masaki_kumamoto_uipath_com/Documents/Documents/UiPath/04_Templates/DocumentUnderstandingEvaluationTemplate/assets/Template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="13_ncr:1_{1831B90B-3A3E-4F89-94DA-EDDB8AC42814}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AA27A138-DE9C-458D-93B1-5DC38926A172}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="13_ncr:1_{1831B90B-3A3E-4F89-94DA-EDDB8AC42814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A70F2D0-7BB5-43DD-80BE-2108A6CFBC6B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6840" yWindow="-16035" windowWidth="35205" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>isMissing</t>
   </si>
@@ -88,12 +88,6 @@
     <t>Set</t>
   </si>
   <si>
-    <t>Table</t>
-  </si>
-  <si>
-    <t>TableColumn</t>
-  </si>
-  <si>
     <t>TableName</t>
   </si>
   <si>
@@ -137,18 +131,6 @@
   </si>
   <si>
     <t>Boolean_Correct</t>
-  </si>
-  <si>
-    <t>Table_Total</t>
-  </si>
-  <si>
-    <t>Table_Correct</t>
-  </si>
-  <si>
-    <t>TableColumn_Total</t>
-  </si>
-  <si>
-    <t>TableColumn_Correct</t>
   </si>
   <si>
     <t>Boolean_Accuracy</t>
@@ -238,63 +220,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -350,10 +276,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{12D40707-6902-402B-A2D7-4390CA2BA40C}" name="Summary" displayName="Summary" ref="B3:X4" insertRow="1" totalsRowShown="0" headerRowDxfId="11">
-  <autoFilter ref="B3:X4" xr:uid="{B9669EFA-0EA3-4114-B365-342FA5C0E038}"/>
-  <tableColumns count="23">
-    <tableColumn id="23" xr3:uid="{A56B4635-0FE8-4013-BD89-83C339961402}" name="TableName" dataDxfId="10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{12D40707-6902-402B-A2D7-4390CA2BA40C}" name="Summary" displayName="Summary" ref="B3:T4" insertRow="1" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="B3:T4" xr:uid="{B9669EFA-0EA3-4114-B365-342FA5C0E038}"/>
+  <tableColumns count="19">
+    <tableColumn id="23" xr3:uid="{A56B4635-0FE8-4013-BD89-83C339961402}" name="TableName" dataDxfId="2"/>
     <tableColumn id="1" xr3:uid="{FDFEA7B6-1840-4996-93CC-77B45743618A}" name="FileName"/>
     <tableColumn id="2" xr3:uid="{11656835-6059-4605-ADE1-84A9F52A2C40}" name="Text_Total">
       <calculatedColumnFormula>COUNTIFS(INDIRECT(Summary[[#This Row],[TableName]] &amp; "[FieldType]"),D$2)</calculatedColumnFormula>
@@ -397,26 +323,14 @@
     <tableColumn id="15" xr3:uid="{C9B1AEDF-5F45-41DC-9329-5698D1AE635E}" name="Boolean_Correct">
       <calculatedColumnFormula>COUNTIFS(INDIRECT(Summary[[#This Row],[TableName]] &amp; "[FieldType]"),Q$2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{DDF8A382-FCC6-4EF7-B177-CE6D66991117}" name="Table_Total">
-      <calculatedColumnFormula>COUNTIFS(INDIRECT(Summary[[#This Row],[TableName]] &amp; "[FieldType]"),R$2)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="17" xr3:uid="{5F94CBB1-19D6-4F43-AE2B-238C0DD57165}" name="Table_Correct">
-      <calculatedColumnFormula>COUNTIFS(INDIRECT(Summary[[#This Row],[TableName]] &amp; "[FieldType]"),S$2)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="18" xr3:uid="{B5FD42CC-EF01-4430-92B8-8A88BE3B291D}" name="TableColumn_Total">
-      <calculatedColumnFormula>COUNTIFS(INDIRECT(Summary[[#This Row],[TableName]] &amp; "[FieldType]"),T$2)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="19" xr3:uid="{EE330A70-4FE9-4709-908E-E49EACB0ED4F}" name="TableColumn_Correct">
-      <calculatedColumnFormula>COUNTIFS(INDIRECT(Summary[[#This Row],[TableName]] &amp; "[FieldType]"),U$2)</calculatedColumnFormula>
-    </tableColumn>
     <tableColumn id="20" xr3:uid="{34CBF333-76E0-4A1E-A766-22839DDE37C8}" name="Boolean_Accuracy" dataCellStyle="Percent">
       <calculatedColumnFormula>Summary[[#This Row],[Boolean_Correct]]/Summary[[#This Row],[Boolean_Total]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="21" xr3:uid="{0D80A7E4-626E-454E-9356-D73F1C9FFF99}" name="Others_Accuracy" dataCellStyle="Percent">
-      <calculatedColumnFormula>SUM(Summary[[#This Row],[Text_Correct]],Summary[[#This Row],[Number_Correct]],Summary[[#This Row],[Date_Correct]],Summary[[#This Row],[Name_Correct]],Summary[[#This Row],[Address_Correct]],Summary[[#This Row],[Set_Correct]],Summary[[#This Row],[Table_Correct]],Summary[[#This Row],[TableColumn_Correct]])/SUM(Summary[[#This Row],[Text_Total]],Summary[[#This Row],[Number_Total]],Summary[[#This Row],[Date_Total]],Summary[[#This Row],[Name_Total]],Summary[[#This Row],[Address_Total]],Summary[[#This Row],[Set_Total]],,Summary[[#This Row],[Table_Total]],Summary[[#This Row],[TableColumn_Total]],Summary[[#This Row],[Boolean_Accuracy]])</calculatedColumnFormula>
+      <calculatedColumnFormula>SUM(Summary[[#This Row],[Text_Correct]],Summary[[#This Row],[Number_Correct]],Summary[[#This Row],[Date_Correct]],Summary[[#This Row],[Name_Correct]],Summary[[#This Row],[Address_Correct]],Summary[[#This Row],[Set_Correct]],#REF!,#REF!)/SUM(Summary[[#This Row],[Text_Total]],Summary[[#This Row],[Number_Total]],Summary[[#This Row],[Date_Total]],Summary[[#This Row],[Name_Total]],Summary[[#This Row],[Address_Total]],Summary[[#This Row],[Set_Total]],,#REF!,#REF!,Summary[[#This Row],[Boolean_Accuracy]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="22" xr3:uid="{3CE65A5D-B36D-4D4F-B678-F9305F990802}" name="Total_Accuracy" dataCellStyle="Percent">
-      <calculatedColumnFormula>SUM(Summary[[#This Row],[Text_Correct]],Summary[[#This Row],[Number_Correct]],Summary[[#This Row],[Date_Correct]],Summary[[#This Row],[Name_Correct]],Summary[[#This Row],[Address_Correct]],Summary[[#This Row],[Set_Correct]],Summary[[#This Row],[Boolean_Correct]],Summary[[#This Row],[Table_Correct]],Summary[[#This Row],[TableColumn_Correct]])/SUM(Summary[[#This Row],[Text_Total]],Summary[[#This Row],[Number_Total]],Summary[[#This Row],[Date_Total]],Summary[[#This Row],[Name_Total]],Summary[[#This Row],[Address_Total]],Summary[[#This Row],[Set_Total]],Summary[[#This Row],[Boolean_Total]],Summary[[#This Row],[Table_Total]],Summary[[#This Row],[TableColumn_Total]],Summary[[#This Row],[Boolean_Accuracy]])</calculatedColumnFormula>
+      <calculatedColumnFormula>SUM(Summary[[#This Row],[Text_Correct]],Summary[[#This Row],[Number_Correct]],Summary[[#This Row],[Date_Correct]],Summary[[#This Row],[Name_Correct]],Summary[[#This Row],[Address_Correct]],Summary[[#This Row],[Set_Correct]],Summary[[#This Row],[Boolean_Correct]],#REF!,#REF!)/SUM(Summary[[#This Row],[Text_Total]],Summary[[#This Row],[Number_Total]],Summary[[#This Row],[Date_Total]],Summary[[#This Row],[Name_Total]],Summary[[#This Row],[Address_Total]],Summary[[#This Row],[Set_Total]],Summary[[#This Row],[Boolean_Total]],#REF!,#REF!,Summary[[#This Row],[Boolean_Accuracy]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -686,7 +600,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BE4FAD5-ED35-4E1A-94DC-5D6A193D9BD8}">
-  <dimension ref="B1:X4"/>
+  <dimension ref="B1:T4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -695,12 +609,12 @@
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
     <col min="3" max="3" width="30.140625" customWidth="1"/>
-    <col min="4" max="21" width="9.28515625" customWidth="1"/>
-    <col min="22" max="24" width="17.42578125" style="9" customWidth="1"/>
+    <col min="4" max="17" width="9.28515625" customWidth="1"/>
+    <col min="18" max="20" width="17.42578125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>11</v>
       </c>
@@ -743,95 +657,71 @@
       <c r="Q2" t="s">
         <v>8</v>
       </c>
-      <c r="R2" t="s">
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="S2" t="s">
-        <v>17</v>
-      </c>
-      <c r="T2" t="s">
-        <v>18</v>
-      </c>
-      <c r="U2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
-        <v>19</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="I3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="J3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="K3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="L3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="M3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="N3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="O3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="P3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="Q3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="R3" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="Q3" s="7" t="s">
+      <c r="S3" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="R3" s="7" t="s">
+      <c r="T3" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="S3" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="T3" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="U3" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="V3" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="W3" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="X3" s="10" t="s">
-        <v>40</v>
-      </c>
     </row>
-    <row r="4" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" s="8"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="V4:X4">
+  <conditionalFormatting sqref="R4:T4">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="formula" val="0"/>
@@ -867,7 +757,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>V4:X4</xm:sqref>
+          <xm:sqref>R4:T4</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Convert to test Template from Process template - Added a Verification Activity
</commit_message>
<xml_diff>
--- a/assets/Template/ReportTemplate.xlsx
+++ b/assets/Template/ReportTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/masaki_kumamoto_uipath_com/Documents/Documents/UiPath/04_Templates/DocumentUnderstandingEvaluationTemplate/assets/Template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/masaki_kumamoto_uipath_com/Documents/Documents/UiPath/04_Templates/DUET/assets/Template/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="74" documentId="13_ncr:1_{1831B90B-3A3E-4F89-94DA-EDDB8AC42814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C3FA590-0A52-4F94-BDE0-B271258574E2}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16155" yWindow="-18360" windowWidth="29265" windowHeight="20295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>

</xml_diff>